<commit_message>
Bold font in each xlsx file
</commit_message>
<xml_diff>
--- a/exp/ablation-PLOJF-12_59/WangJianFolder/expResult/2025-9-12/PLOJF-12_59/PLOJF.xlsx
+++ b/exp/ablation-PLOJF-12_59/WangJianFolder/expResult/2025-9-12/PLOJF-12_59/PLOJF.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PLOJF-25-9-15\exp\ablation-PLOJF-12_59\WangJianFolder\expResult\2025-9-12\PLOJF-12_59\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FB4DBD-8C17-431C-8A39-7ED9838756AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5B2437-074E-4D8E-B7B6-8FF5C7D46EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="540" windowWidth="14520" windowHeight="15660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="420" windowWidth="29040" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cmpResult" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1849" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="134">
   <si>
     <t>Func</t>
   </si>
@@ -461,10 +461,24 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000E+00"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -493,9 +507,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -810,10 +828,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F62"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -851,16 +870,16 @@
       <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>1730.26131400899</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
         <v>21934.647496407055</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="5">
         <v>1959.8576585996525</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="5">
         <v>10353.596534923305</v>
       </c>
     </row>
@@ -868,16 +887,16 @@
       <c r="B3" t="s">
         <v>34</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>1323.9442874602521</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>6659.5008137032755</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="5">
         <v>1374.5198909103297</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="5">
         <v>1982.4462273940305</v>
       </c>
     </row>
@@ -888,16 +907,16 @@
       <c r="B4" t="s">
         <v>33</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>4102.8482699021542</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>3971.2026534662996</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>3844.0039922219798</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="5">
         <v>24366.815744708965</v>
       </c>
     </row>
@@ -905,16 +924,16 @@
       <c r="B5" t="s">
         <v>34</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>1273.5587275434339</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>1459.3506208526894</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <v>1322.3872443980981</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="5">
         <v>5523.1090226173146</v>
       </c>
     </row>
@@ -925,16 +944,16 @@
       <c r="B6" t="s">
         <v>33</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>487.86121936821706</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>491.38409794943618</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="5">
         <v>486.22544758736586</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="4">
         <v>470.92698552605054</v>
       </c>
     </row>
@@ -942,16 +961,16 @@
       <c r="B7" t="s">
         <v>34</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="5">
         <v>19.025745877071177</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <v>16.511604564517157</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="5">
         <v>16.544905121142097</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="5">
         <v>16.839120397853037</v>
       </c>
     </row>
@@ -962,16 +981,16 @@
       <c r="B8" t="s">
         <v>33</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>535.94277609029814</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <v>535.3066277982058</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="5">
         <v>536.70992581466396</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="5">
         <v>551.29800603326112</v>
       </c>
     </row>
@@ -979,16 +998,16 @@
       <c r="B9" t="s">
         <v>34</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="5">
         <v>10.968575767109623</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>7.3747296263630195</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="5">
         <v>8.8772232866586798</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="5">
         <v>8.7525245576868933</v>
       </c>
     </row>
@@ -999,16 +1018,16 @@
       <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>600.97116882382397</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
         <v>600.86463275954998</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="4">
         <v>600.86405794036955</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="5">
         <v>604.38381426940407</v>
       </c>
     </row>
@@ -1016,16 +1035,16 @@
       <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <v>0.43908660373225811</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <v>0.27021064255468308</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <v>0.39697450342156959</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="5">
         <v>1.0771803784837304</v>
       </c>
     </row>
@@ -1036,16 +1055,16 @@
       <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>757.92894167255486</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="5">
         <v>759.09387484076046</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="4">
         <v>757.58065830244846</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="5">
         <v>821.39183141272224</v>
       </c>
     </row>
@@ -1053,16 +1072,16 @@
       <c r="B13" t="s">
         <v>34</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <v>9.664331968545282</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <v>7.3331876819790827</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="5">
         <v>9.1921768996461708</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="5">
         <v>16.623902653343638</v>
       </c>
     </row>
@@ -1073,16 +1092,16 @@
       <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="5">
         <v>838.2672651707403</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="5">
         <v>837.71745573129658</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="4">
         <v>837.09444752738875</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="5">
         <v>849.16218611826037</v>
       </c>
     </row>
@@ -1090,16 +1109,16 @@
       <c r="B15" t="s">
         <v>34</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="5">
         <v>9.5598585503723363</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="5">
         <v>8.3749493131299353</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="5">
         <v>8.1305549914702464</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="4">
         <v>7.5872946013476703</v>
       </c>
     </row>
@@ -1110,16 +1129,16 @@
       <c r="B16" t="s">
         <v>33</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="5">
         <v>924.94140369703985</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="4">
         <v>920.30132725714304</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="5">
         <v>923.47211089461371</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="5">
         <v>1317.9022909562893</v>
       </c>
     </row>
@@ -1127,16 +1146,16 @@
       <c r="B17" t="s">
         <v>34</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="5">
         <v>16.917183303304459</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="4">
         <v>14.509659839672047</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="5">
         <v>14.976866661616873</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="5">
         <v>131.73923116721156</v>
       </c>
     </row>
@@ -1147,16 +1166,16 @@
       <c r="B18" t="s">
         <v>33</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="5">
         <v>3033.6666764386459</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="5">
         <v>3072.6478006055945</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="5">
         <v>3006.7654583087224</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="4">
         <v>3004.2507321019202</v>
       </c>
     </row>
@@ -1164,16 +1183,16 @@
       <c r="B19" t="s">
         <v>34</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="5">
         <v>326.53849385047869</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="4">
         <v>268.79392729308097</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="5">
         <v>307.01042062502341</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="5">
         <v>295.11424673674685</v>
       </c>
     </row>
@@ -1184,16 +1203,16 @@
       <c r="B20" t="s">
         <v>33</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="4">
         <v>1143.0929577351642</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="5">
         <v>1145.025509717364</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="5">
         <v>1152.2914851842957</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="5">
         <v>1182.4594829924292</v>
       </c>
     </row>
@@ -1201,16 +1220,16 @@
       <c r="B21" t="s">
         <v>34</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="4">
         <v>9.9887961026629579</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="5">
         <v>10.735675034530608</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="5">
         <v>16.855181435328625</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="5">
         <v>19.357146226667471</v>
       </c>
     </row>
@@ -1221,16 +1240,16 @@
       <c r="B22" t="s">
         <v>33</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="4">
         <v>38702.409908438174</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="5">
         <v>61857.002769903163</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="5">
         <v>55334.873107154199</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="5">
         <v>835861.90568216599</v>
       </c>
     </row>
@@ -1238,16 +1257,16 @@
       <c r="B23" t="s">
         <v>34</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="4">
         <v>38963.957944795518</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="5">
         <v>74995.714168097024</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="5">
         <v>70319.481006075497</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="5">
         <v>854631.57311942684</v>
       </c>
     </row>
@@ -1258,16 +1277,16 @@
       <c r="B24" t="s">
         <v>33</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="4">
         <v>2842.4051007306448</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="5">
         <v>2904.9476944245716</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="5">
         <v>3152.4275239880544</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="5">
         <v>6996.7000245717927</v>
       </c>
     </row>
@@ -1275,16 +1294,16 @@
       <c r="B25" t="s">
         <v>34</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="5">
         <v>549.14164134443956</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="4">
         <v>433.6993240061812</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="5">
         <v>608.72579579241471</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="5">
         <v>1791.5237313883033</v>
       </c>
     </row>
@@ -1295,16 +1314,16 @@
       <c r="B26" t="s">
         <v>33</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="5">
         <v>1662.1873759455068</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="4">
         <v>1648.2535575051675</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="5">
         <v>1654.7467830727003</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="5">
         <v>2643.6829523105557</v>
       </c>
     </row>
@@ -1312,16 +1331,16 @@
       <c r="B27" t="s">
         <v>34</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="5">
         <v>66.18327247235267</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="4">
         <v>52.069964516823347</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="5">
         <v>60.906062998145266</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="5">
         <v>893.99144571413547</v>
       </c>
     </row>
@@ -1332,16 +1351,16 @@
       <c r="B28" t="s">
         <v>33</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="5">
         <v>1888.1294333471103</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="4">
         <v>1878.2446537231517</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="5">
         <v>1898.2276585983718</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="5">
         <v>4052.5809998457257</v>
       </c>
     </row>
@@ -1349,16 +1368,16 @@
       <c r="B29" t="s">
         <v>34</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="5">
         <v>173.64930714708709</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="5">
         <v>167.09117639182406</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="4">
         <v>122.82262073260057</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="5">
         <v>942.56403578660593</v>
       </c>
     </row>
@@ -1369,16 +1388,16 @@
       <c r="B30" t="s">
         <v>33</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="5">
         <v>1930.8011932010336</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="5">
         <v>1962.1683425400306</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="5">
         <v>1936.9023165683607</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="4">
         <v>1888.2721716865199</v>
       </c>
     </row>
@@ -1386,16 +1405,16 @@
       <c r="B31" t="s">
         <v>34</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="5">
         <v>117.68537503416292</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="5">
         <v>142.5048664242058</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="5">
         <v>133.28258677911978</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="4">
         <v>96.586569116910368</v>
       </c>
     </row>
@@ -1406,16 +1425,16 @@
       <c r="B32" t="s">
         <v>33</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="5">
         <v>1828.2507493789028</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="4">
         <v>1819.6551857088048</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="5">
         <v>1830.5434244466267</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="5">
         <v>1842.1794635079682</v>
       </c>
     </row>
@@ -1423,16 +1442,16 @@
       <c r="B33" t="s">
         <v>34</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="5">
         <v>26.900743544095487</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="4">
         <v>24.278292660960297</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="5">
         <v>34.986910613021145</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="5">
         <v>36.552507770680243</v>
       </c>
     </row>
@@ -1443,16 +1462,16 @@
       <c r="B34" t="s">
         <v>33</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="5">
         <v>9770.8875931016046</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="5">
         <v>9814.5036705164803</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="4">
         <v>9468.5026864930569</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="5">
         <v>79841.413565268333</v>
       </c>
     </row>
@@ -1460,16 +1479,16 @@
       <c r="B35" t="s">
         <v>34</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="5">
         <v>5465.784894092606</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="4">
         <v>4278.1938409352051</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="5">
         <v>5111.1928508192914</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="5">
         <v>37125.890914137119</v>
       </c>
     </row>
@@ -1480,16 +1499,16 @@
       <c r="B36" t="s">
         <v>33</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="4">
         <v>2001.1650811528857</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="5">
         <v>2002.8968291984972</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="5">
         <v>2009.1404748346336</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="5">
         <v>2280.0907047214109</v>
       </c>
     </row>
@@ -1497,16 +1516,16 @@
       <c r="B37" t="s">
         <v>34</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="5">
         <v>22.840356812857681</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="4">
         <v>20.801378157813012</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="5">
         <v>23.600728085154977</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="5">
         <v>134.17500573121703</v>
       </c>
     </row>
@@ -1517,16 +1536,16 @@
       <c r="B38" t="s">
         <v>33</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="5">
         <v>2171.3686788010473</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="5">
         <v>2165.9523408964942</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="4">
         <v>2156.1956080173641</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="5">
         <v>2203.2352113342258</v>
       </c>
     </row>
@@ -1534,16 +1553,16 @@
       <c r="B39" t="s">
         <v>34</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="5">
         <v>37.518256216460692</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="5">
         <v>52.003923691013654</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="4">
         <v>31.179988062022975</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="5">
         <v>53.927293179653653</v>
       </c>
     </row>
@@ -1554,16 +1573,16 @@
       <c r="B40" t="s">
         <v>33</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="4">
         <v>2200.0023791112044</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="5">
         <v>2200.0108073569795</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="5">
         <v>2200.0028648259472</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="5">
         <v>2200.0068694607671</v>
       </c>
     </row>
@@ -1571,16 +1590,16 @@
       <c r="B41" t="s">
         <v>34</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="5">
         <v>8.2389989103433963E-4</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="5">
         <v>1.972099456471612E-3</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="5">
         <v>1.339077542884272E-3</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="4">
         <v>5.7896961919447806E-4</v>
       </c>
     </row>
@@ -1591,16 +1610,16 @@
       <c r="B42" t="s">
         <v>33</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="5">
         <v>2300.002727640504</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="5">
         <v>2300.0109869438106</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="4">
         <v>2300.0024303237415</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="5">
         <v>2300.0070298778965</v>
       </c>
     </row>
@@ -1608,16 +1627,16 @@
       <c r="B43" t="s">
         <v>34</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="5">
         <v>1.2011112457484959E-3</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="5">
         <v>1.9041837144584846E-3</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="5">
         <v>1.0718559101145317E-3</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="4">
         <v>6.7509277509934221E-4</v>
       </c>
     </row>
@@ -1628,16 +1647,16 @@
       <c r="B44" t="s">
         <v>33</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="5">
         <v>2832.1909695071013</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="4">
         <v>2831.0245537353253</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="5">
         <v>2834.5245478166439</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="5">
         <v>2835.2361947018567</v>
       </c>
     </row>
@@ -1645,16 +1664,16 @@
       <c r="B45" t="s">
         <v>34</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="5">
         <v>13.706999979309513</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="5">
         <v>12.436104123942087</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="5">
         <v>10.174646899365214</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="4">
         <v>9.4949649135044236</v>
       </c>
     </row>
@@ -1665,16 +1684,16 @@
       <c r="B46" t="s">
         <v>33</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="5">
         <v>2702.0210771188022</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="5">
         <v>2701.9956058553344</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="4">
         <v>2701.9071240704911</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="5">
         <v>3388.7108152070591</v>
       </c>
     </row>
@@ -1682,16 +1701,16 @@
       <c r="B47" t="s">
         <v>34</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="5">
         <v>0.3206258634919571</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="4">
         <v>0.27057104036406882</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="5">
         <v>0.36654292705563696</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="5">
         <v>7.5886119432393642</v>
       </c>
     </row>
@@ -1702,16 +1721,16 @@
       <c r="B48" t="s">
         <v>33</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="5">
         <v>2908.680029824855</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="5">
         <v>2908.2222746945135</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="5">
         <v>2910.0181926222567</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="4">
         <v>2903.1410290335357</v>
       </c>
     </row>
@@ -1719,16 +1738,16 @@
       <c r="B49" t="s">
         <v>34</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="5">
         <v>8.9419857000711254</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="5">
         <v>7.284795017941569</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="5">
         <v>8.3937967270070857</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="4">
         <v>4.3674474447989802</v>
       </c>
     </row>
@@ -1739,16 +1758,16 @@
       <c r="B50" t="s">
         <v>33</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="5">
         <v>4789.220367008671</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="5">
         <v>4723.7984468307577</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="5">
         <v>4768.6162582674597</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="4">
         <v>4522.3415207909866</v>
       </c>
     </row>
@@ -1756,16 +1775,16 @@
       <c r="B51" t="s">
         <v>34</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="4">
         <v>104.84380474140374</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="5">
         <v>375.05488393616787</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="5">
         <v>113.18851428338468</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="5">
         <v>653.03626597584696</v>
       </c>
     </row>
@@ -1776,16 +1795,16 @@
       <c r="B52" t="s">
         <v>33</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="5">
         <v>3487.1940896629117</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="5">
         <v>3499.9768467506792</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="5">
         <v>3507.8755686977979</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="4">
         <v>3437.9121909343467</v>
       </c>
     </row>
@@ -1793,16 +1812,16 @@
       <c r="B53" t="s">
         <v>34</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="5">
         <v>34.760254524772897</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="5">
         <v>27.371796399639795</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="5">
         <v>40.333136244737311</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="4">
         <v>18.448554453562686</v>
       </c>
     </row>
@@ -1813,16 +1832,16 @@
       <c r="B54" t="s">
         <v>33</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="4">
         <v>3221.7762057180385</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="5">
         <v>3231.2304351365779</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="5">
         <v>3223.8532487911789</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="5">
         <v>3234.785653591608</v>
       </c>
     </row>
@@ -1830,16 +1849,16 @@
       <c r="B55" t="s">
         <v>34</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="5">
         <v>53.346548573620723</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="5">
         <v>41.562400477450822</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="5">
         <v>43.692482942734117</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="4">
         <v>22.368365960239732</v>
       </c>
     </row>
@@ -1850,16 +1869,16 @@
       <c r="B56" t="s">
         <v>33</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="5">
         <v>3397.5006464511544</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="5">
         <v>3412.1929987105259</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="5">
         <v>3426.2306889435581</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="4">
         <v>3382.156529187384</v>
       </c>
     </row>
@@ -1867,16 +1886,16 @@
       <c r="B57" t="s">
         <v>34</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="5">
         <v>62.772677790029647</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="5">
         <v>60.554361532982561</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="5">
         <v>54.964988938352917</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="4">
         <v>52.750128452935591</v>
       </c>
     </row>
@@ -1887,16 +1906,16 @@
       <c r="B58" t="s">
         <v>33</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="5">
         <v>14535.638121548025</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="4">
         <v>11874.260143647352</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="5">
         <v>12233.965922277514</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="5">
         <v>51505.542266634395</v>
       </c>
     </row>
@@ -1904,16 +1923,16 @@
       <c r="B59" t="s">
         <v>34</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="5">
         <v>7527.1596740659643</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="5">
         <v>3863.2157726453443</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="4">
         <v>3412.575588593359</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="5">
         <v>20131.106921354283</v>
       </c>
     </row>
@@ -1921,16 +1940,16 @@
       <c r="A60" t="s">
         <v>30</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" s="3" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1938,37 +1957,17 @@
       <c r="A61" t="s">
         <v>31</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="3" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" t="s">
-        <v>0</v>
-      </c>
-      <c r="B62" t="s">
-        <v>32</v>
-      </c>
-      <c r="C62" t="s">
-        <v>35</v>
-      </c>
-      <c r="D62" t="s">
-        <v>38</v>
-      </c>
-      <c r="E62" t="s">
-        <v>41</v>
-      </c>
-      <c r="F62" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1978,6 +1977,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2522,6 +2522,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3066,6 +3067,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3610,6 +3612,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4154,6 +4157,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4698,6 +4702,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5242,6 +5247,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5786,6 +5792,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6330,6 +6337,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6874,6 +6882,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7418,6 +7427,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7857,6 +7867,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8401,6 +8412,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8945,6 +8957,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+  <sheetPr codeName="Sheet22"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9489,6 +9502,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <sheetPr codeName="Sheet23"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10033,6 +10047,7 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <sheetPr codeName="Sheet24"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10577,6 +10592,7 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+  <sheetPr codeName="Sheet25"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11121,6 +11137,7 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+  <sheetPr codeName="Sheet26"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11665,6 +11682,7 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+  <sheetPr codeName="Sheet27"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12209,6 +12227,7 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+  <sheetPr codeName="Sheet28"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12753,6 +12772,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+  <sheetPr codeName="Sheet29"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13297,9 +13317,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
@@ -14553,6 +14574,7 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+  <sheetPr codeName="Sheet30"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -15097,6 +15119,7 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+  <sheetPr codeName="Sheet31"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -15641,6 +15664,7 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+  <sheetPr codeName="Sheet32"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -16185,6 +16209,7 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+  <sheetPr codeName="Sheet33"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -16729,6 +16754,7 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{276FD02B-85B4-440B-9241-D14B98290E32}">
+  <sheetPr codeName="Sheet34"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -16741,6 +16767,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -17472,6 +17499,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -18016,6 +18044,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -18560,6 +18589,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -19104,6 +19134,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -19648,6 +19679,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Upload initial hand writing version of PLOJF (only benchmark section)
</commit_message>
<xml_diff>
--- a/exp/ablation-PLOJF-12_59/WangJianFolder/expResult/2025-9-12/PLOJF-12_59/PLOJF.xlsx
+++ b/exp/ablation-PLOJF-12_59/WangJianFolder/expResult/2025-9-12/PLOJF-12_59/PLOJF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PLOJF-25-9-15\exp\ablation-PLOJF-12_59\WangJianFolder\expResult\2025-9-12\PLOJF-12_59\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5B2437-074E-4D8E-B7B6-8FF5C7D46EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5057124-E66D-4D72-AD67-12D184A99084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="420" windowWidth="29040" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="420" windowWidth="29040" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cmpResult" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1934" uniqueCount="134">
   <si>
     <t>Func</t>
   </si>
@@ -464,21 +464,26 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -507,13 +512,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -829,45 +835,85 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:BO61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K60" sqref="K60"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51:J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" customWidth="1"/>
-    <col min="3" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="3"/>
+    <col min="10" max="11" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="24" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="33" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="39" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="42" max="43" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="57" max="58" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="62" max="63" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="68" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
+    <row r="1" spans="1:67">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+    <row r="2" spans="1:67">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="4">
@@ -882,9 +928,96 @@
       <c r="F2" s="5">
         <v>10353.596534923305</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="B3" t="s">
+      <c r="J2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="BD2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="BF2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="BH2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="BJ2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="BL2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="BN2" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:67">
+      <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="4">
@@ -899,12 +1032,186 @@
       <c r="F3" s="5">
         <v>1982.4462273940305</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="J3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AP3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AQ3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AR3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AS3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AT3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AU3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AV3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AW3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AX3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AZ3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="BB3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="BD3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="BE3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="BF3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="BG3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="BH3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="BI3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="BJ3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="BK3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="BL3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="BM3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="BN3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="BO3" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:67">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="5">
@@ -919,9 +1226,183 @@
       <c r="F4" s="5">
         <v>24366.815744708965</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="B5" t="s">
+      <c r="J4" s="4">
+        <v>1730.26131400899</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1323.9442874602521</v>
+      </c>
+      <c r="L4" s="5">
+        <v>4102.8482699021542</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1273.5587275434339</v>
+      </c>
+      <c r="N4" s="5">
+        <v>487.86121936821706</v>
+      </c>
+      <c r="O4" s="5">
+        <v>19.025745877071177</v>
+      </c>
+      <c r="P4" s="5">
+        <v>535.94277609029814</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>10.968575767109623</v>
+      </c>
+      <c r="R4" s="5">
+        <v>600.97116882382397</v>
+      </c>
+      <c r="S4" s="5">
+        <v>0.43908660373225811</v>
+      </c>
+      <c r="T4" s="5">
+        <v>757.92894167255486</v>
+      </c>
+      <c r="U4" s="5">
+        <v>9.664331968545282</v>
+      </c>
+      <c r="V4" s="5">
+        <v>838.2672651707403</v>
+      </c>
+      <c r="W4" s="5">
+        <v>9.5598585503723363</v>
+      </c>
+      <c r="X4" s="5">
+        <v>924.94140369703985</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>16.917183303304459</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>3033.6666764386459</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>326.53849385047869</v>
+      </c>
+      <c r="AB4" s="4">
+        <v>1143.0929577351642</v>
+      </c>
+      <c r="AC4" s="4">
+        <v>9.9887961026629579</v>
+      </c>
+      <c r="AD4" s="4">
+        <v>38702.409908438174</v>
+      </c>
+      <c r="AE4" s="4">
+        <v>38963.957944795518</v>
+      </c>
+      <c r="AF4" s="4">
+        <v>2842.4051007306448</v>
+      </c>
+      <c r="AG4" s="5">
+        <v>549.14164134443956</v>
+      </c>
+      <c r="AH4" s="5">
+        <v>1662.1873759455068</v>
+      </c>
+      <c r="AI4" s="5">
+        <v>66.18327247235267</v>
+      </c>
+      <c r="AJ4" s="5">
+        <v>1888.1294333471103</v>
+      </c>
+      <c r="AK4" s="5">
+        <v>173.64930714708709</v>
+      </c>
+      <c r="AL4" s="5">
+        <v>1930.8011932010336</v>
+      </c>
+      <c r="AM4" s="5">
+        <v>117.68537503416292</v>
+      </c>
+      <c r="AN4" s="5">
+        <v>1828.2507493789028</v>
+      </c>
+      <c r="AO4" s="5">
+        <v>26.900743544095487</v>
+      </c>
+      <c r="AP4" s="5">
+        <v>9770.8875931016046</v>
+      </c>
+      <c r="AQ4" s="5">
+        <v>5465.784894092606</v>
+      </c>
+      <c r="AR4" s="4">
+        <v>2001.1650811528857</v>
+      </c>
+      <c r="AS4" s="5">
+        <v>22.840356812857681</v>
+      </c>
+      <c r="AT4" s="5">
+        <v>2171.3686788010473</v>
+      </c>
+      <c r="AU4" s="5">
+        <v>37.518256216460692</v>
+      </c>
+      <c r="AV4" s="4">
+        <v>2200.0023791112044</v>
+      </c>
+      <c r="AW4" s="5">
+        <v>8.2389989103433963E-4</v>
+      </c>
+      <c r="AX4" s="5">
+        <v>2300.002727640504</v>
+      </c>
+      <c r="AY4" s="5">
+        <v>1.2011112457484959E-3</v>
+      </c>
+      <c r="AZ4" s="5">
+        <v>2832.1909695071013</v>
+      </c>
+      <c r="BA4" s="5">
+        <v>13.706999979309513</v>
+      </c>
+      <c r="BB4" s="5">
+        <v>2702.0210771188022</v>
+      </c>
+      <c r="BC4" s="5">
+        <v>0.3206258634919571</v>
+      </c>
+      <c r="BD4" s="5">
+        <v>2908.680029824855</v>
+      </c>
+      <c r="BE4" s="5">
+        <v>8.9419857000711254</v>
+      </c>
+      <c r="BF4" s="5">
+        <v>4789.220367008671</v>
+      </c>
+      <c r="BG4" s="4">
+        <v>104.84380474140374</v>
+      </c>
+      <c r="BH4" s="5">
+        <v>3487.1940896629117</v>
+      </c>
+      <c r="BI4" s="5">
+        <v>34.760254524772897</v>
+      </c>
+      <c r="BJ4" s="4">
+        <v>3221.7762057180385</v>
+      </c>
+      <c r="BK4" s="5">
+        <v>53.346548573620723</v>
+      </c>
+      <c r="BL4" s="5">
+        <v>3397.5006464511544</v>
+      </c>
+      <c r="BM4" s="5">
+        <v>62.772677790029647</v>
+      </c>
+      <c r="BN4" s="5">
+        <v>14535.638121548025</v>
+      </c>
+      <c r="BO4" s="5">
+        <v>7527.1596740659643</v>
+      </c>
+    </row>
+    <row r="5" spans="1:67">
+      <c r="B5" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="4">
@@ -936,12 +1417,186 @@
       <c r="F5" s="5">
         <v>5523.1090226173146</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
+      <c r="J5" s="5">
+        <v>21934.647496407055</v>
+      </c>
+      <c r="K5" s="5">
+        <v>6659.5008137032755</v>
+      </c>
+      <c r="L5" s="5">
+        <v>3971.2026534662996</v>
+      </c>
+      <c r="M5" s="5">
+        <v>1459.3506208526894</v>
+      </c>
+      <c r="N5" s="5">
+        <v>491.38409794943618</v>
+      </c>
+      <c r="O5" s="4">
+        <v>16.511604564517157</v>
+      </c>
+      <c r="P5" s="4">
+        <v>535.3066277982058</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>7.3747296263630195</v>
+      </c>
+      <c r="R5" s="5">
+        <v>600.86463275954998</v>
+      </c>
+      <c r="S5" s="4">
+        <v>0.27021064255468308</v>
+      </c>
+      <c r="T5" s="5">
+        <v>759.09387484076046</v>
+      </c>
+      <c r="U5" s="4">
+        <v>7.3331876819790827</v>
+      </c>
+      <c r="V5" s="5">
+        <v>837.71745573129658</v>
+      </c>
+      <c r="W5" s="5">
+        <v>8.3749493131299353</v>
+      </c>
+      <c r="X5" s="4">
+        <v>920.30132725714304</v>
+      </c>
+      <c r="Y5" s="4">
+        <v>14.509659839672047</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>3072.6478006055945</v>
+      </c>
+      <c r="AA5" s="4">
+        <v>268.79392729308097</v>
+      </c>
+      <c r="AB5" s="5">
+        <v>1145.025509717364</v>
+      </c>
+      <c r="AC5" s="5">
+        <v>10.735675034530608</v>
+      </c>
+      <c r="AD5" s="5">
+        <v>61857.002769903163</v>
+      </c>
+      <c r="AE5" s="5">
+        <v>74995.714168097024</v>
+      </c>
+      <c r="AF5" s="5">
+        <v>2904.9476944245716</v>
+      </c>
+      <c r="AG5" s="4">
+        <v>433.6993240061812</v>
+      </c>
+      <c r="AH5" s="4">
+        <v>1648.2535575051675</v>
+      </c>
+      <c r="AI5" s="4">
+        <v>52.069964516823347</v>
+      </c>
+      <c r="AJ5" s="4">
+        <v>1878.2446537231517</v>
+      </c>
+      <c r="AK5" s="5">
+        <v>167.09117639182406</v>
+      </c>
+      <c r="AL5" s="5">
+        <v>1962.1683425400306</v>
+      </c>
+      <c r="AM5" s="5">
+        <v>142.5048664242058</v>
+      </c>
+      <c r="AN5" s="4">
+        <v>1819.6551857088048</v>
+      </c>
+      <c r="AO5" s="4">
+        <v>24.278292660960297</v>
+      </c>
+      <c r="AP5" s="5">
+        <v>9814.5036705164803</v>
+      </c>
+      <c r="AQ5" s="4">
+        <v>4278.1938409352051</v>
+      </c>
+      <c r="AR5" s="5">
+        <v>2002.8968291984972</v>
+      </c>
+      <c r="AS5" s="4">
+        <v>20.801378157813012</v>
+      </c>
+      <c r="AT5" s="5">
+        <v>2165.9523408964942</v>
+      </c>
+      <c r="AU5" s="5">
+        <v>52.003923691013654</v>
+      </c>
+      <c r="AV5" s="5">
+        <v>2200.0108073569795</v>
+      </c>
+      <c r="AW5" s="5">
+        <v>1.972099456471612E-3</v>
+      </c>
+      <c r="AX5" s="5">
+        <v>2300.0109869438106</v>
+      </c>
+      <c r="AY5" s="5">
+        <v>1.9041837144584846E-3</v>
+      </c>
+      <c r="AZ5" s="4">
+        <v>2831.0245537353253</v>
+      </c>
+      <c r="BA5" s="5">
+        <v>12.436104123942087</v>
+      </c>
+      <c r="BB5" s="5">
+        <v>2701.9956058553344</v>
+      </c>
+      <c r="BC5" s="4">
+        <v>0.27057104036406882</v>
+      </c>
+      <c r="BD5" s="5">
+        <v>2908.2222746945135</v>
+      </c>
+      <c r="BE5" s="5">
+        <v>7.284795017941569</v>
+      </c>
+      <c r="BF5" s="5">
+        <v>4723.7984468307577</v>
+      </c>
+      <c r="BG5" s="5">
+        <v>375.05488393616787</v>
+      </c>
+      <c r="BH5" s="5">
+        <v>3499.9768467506792</v>
+      </c>
+      <c r="BI5" s="5">
+        <v>27.371796399639795</v>
+      </c>
+      <c r="BJ5" s="5">
+        <v>3231.2304351365779</v>
+      </c>
+      <c r="BK5" s="5">
+        <v>41.562400477450822</v>
+      </c>
+      <c r="BL5" s="5">
+        <v>3412.1929987105259</v>
+      </c>
+      <c r="BM5" s="5">
+        <v>60.554361532982561</v>
+      </c>
+      <c r="BN5" s="4">
+        <v>11874.260143647352</v>
+      </c>
+      <c r="BO5" s="5">
+        <v>3863.2157726453443</v>
+      </c>
+    </row>
+    <row r="6" spans="1:67">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="5">
@@ -956,9 +1611,183 @@
       <c r="F6" s="4">
         <v>470.92698552605054</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="B7" t="s">
+      <c r="J6" s="5">
+        <v>1959.8576585996525</v>
+      </c>
+      <c r="K6" s="5">
+        <v>1374.5198909103297</v>
+      </c>
+      <c r="L6" s="4">
+        <v>3844.0039922219798</v>
+      </c>
+      <c r="M6" s="5">
+        <v>1322.3872443980981</v>
+      </c>
+      <c r="N6" s="5">
+        <v>486.22544758736586</v>
+      </c>
+      <c r="O6" s="5">
+        <v>16.544905121142097</v>
+      </c>
+      <c r="P6" s="5">
+        <v>536.70992581466396</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>8.8772232866586798</v>
+      </c>
+      <c r="R6" s="4">
+        <v>600.86405794036955</v>
+      </c>
+      <c r="S6" s="5">
+        <v>0.39697450342156959</v>
+      </c>
+      <c r="T6" s="4">
+        <v>757.58065830244846</v>
+      </c>
+      <c r="U6" s="5">
+        <v>9.1921768996461708</v>
+      </c>
+      <c r="V6" s="4">
+        <v>837.09444752738875</v>
+      </c>
+      <c r="W6" s="5">
+        <v>8.1305549914702464</v>
+      </c>
+      <c r="X6" s="5">
+        <v>923.47211089461371</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>14.976866661616873</v>
+      </c>
+      <c r="Z6" s="5">
+        <v>3006.7654583087224</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>307.01042062502341</v>
+      </c>
+      <c r="AB6" s="5">
+        <v>1152.2914851842957</v>
+      </c>
+      <c r="AC6" s="5">
+        <v>16.855181435328625</v>
+      </c>
+      <c r="AD6" s="5">
+        <v>55334.873107154199</v>
+      </c>
+      <c r="AE6" s="5">
+        <v>70319.481006075497</v>
+      </c>
+      <c r="AF6" s="5">
+        <v>3152.4275239880544</v>
+      </c>
+      <c r="AG6" s="5">
+        <v>608.72579579241471</v>
+      </c>
+      <c r="AH6" s="5">
+        <v>1654.7467830727003</v>
+      </c>
+      <c r="AI6" s="5">
+        <v>60.906062998145266</v>
+      </c>
+      <c r="AJ6" s="5">
+        <v>1898.2276585983718</v>
+      </c>
+      <c r="AK6" s="4">
+        <v>122.82262073260057</v>
+      </c>
+      <c r="AL6" s="5">
+        <v>1936.9023165683607</v>
+      </c>
+      <c r="AM6" s="5">
+        <v>133.28258677911978</v>
+      </c>
+      <c r="AN6" s="5">
+        <v>1830.5434244466267</v>
+      </c>
+      <c r="AO6" s="5">
+        <v>34.986910613021145</v>
+      </c>
+      <c r="AP6" s="4">
+        <v>9468.5026864930569</v>
+      </c>
+      <c r="AQ6" s="5">
+        <v>5111.1928508192914</v>
+      </c>
+      <c r="AR6" s="5">
+        <v>2009.1404748346336</v>
+      </c>
+      <c r="AS6" s="5">
+        <v>23.600728085154977</v>
+      </c>
+      <c r="AT6" s="4">
+        <v>2156.1956080173641</v>
+      </c>
+      <c r="AU6" s="4">
+        <v>31.179988062022975</v>
+      </c>
+      <c r="AV6" s="5">
+        <v>2200.0028648259472</v>
+      </c>
+      <c r="AW6" s="5">
+        <v>1.339077542884272E-3</v>
+      </c>
+      <c r="AX6" s="4">
+        <v>2300.0024303237415</v>
+      </c>
+      <c r="AY6" s="5">
+        <v>1.0718559101145317E-3</v>
+      </c>
+      <c r="AZ6" s="5">
+        <v>2834.5245478166439</v>
+      </c>
+      <c r="BA6" s="5">
+        <v>10.174646899365214</v>
+      </c>
+      <c r="BB6" s="4">
+        <v>2701.9071240704911</v>
+      </c>
+      <c r="BC6" s="5">
+        <v>0.36654292705563696</v>
+      </c>
+      <c r="BD6" s="5">
+        <v>2910.0181926222567</v>
+      </c>
+      <c r="BE6" s="5">
+        <v>8.3937967270070857</v>
+      </c>
+      <c r="BF6" s="5">
+        <v>4768.6162582674597</v>
+      </c>
+      <c r="BG6" s="5">
+        <v>113.18851428338468</v>
+      </c>
+      <c r="BH6" s="5">
+        <v>3507.8755686977979</v>
+      </c>
+      <c r="BI6" s="5">
+        <v>40.333136244737311</v>
+      </c>
+      <c r="BJ6" s="5">
+        <v>3223.8532487911789</v>
+      </c>
+      <c r="BK6" s="5">
+        <v>43.692482942734117</v>
+      </c>
+      <c r="BL6" s="5">
+        <v>3426.2306889435581</v>
+      </c>
+      <c r="BM6" s="5">
+        <v>54.964988938352917</v>
+      </c>
+      <c r="BN6" s="5">
+        <v>12233.965922277514</v>
+      </c>
+      <c r="BO6" s="4">
+        <v>3412.575588593359</v>
+      </c>
+    </row>
+    <row r="7" spans="1:67">
+      <c r="B7" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="5">
@@ -973,12 +1802,186 @@
       <c r="F7" s="5">
         <v>16.839120397853037</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
+      <c r="J7" s="5">
+        <v>10353.596534923305</v>
+      </c>
+      <c r="K7" s="5">
+        <v>1982.4462273940305</v>
+      </c>
+      <c r="L7" s="5">
+        <v>24366.815744708965</v>
+      </c>
+      <c r="M7" s="5">
+        <v>5523.1090226173146</v>
+      </c>
+      <c r="N7" s="4">
+        <v>470.92698552605054</v>
+      </c>
+      <c r="O7" s="5">
+        <v>16.839120397853037</v>
+      </c>
+      <c r="P7" s="5">
+        <v>551.29800603326112</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>8.7525245576868933</v>
+      </c>
+      <c r="R7" s="5">
+        <v>604.38381426940407</v>
+      </c>
+      <c r="S7" s="5">
+        <v>1.0771803784837304</v>
+      </c>
+      <c r="T7" s="5">
+        <v>821.39183141272224</v>
+      </c>
+      <c r="U7" s="5">
+        <v>16.623902653343638</v>
+      </c>
+      <c r="V7" s="5">
+        <v>849.16218611826037</v>
+      </c>
+      <c r="W7" s="4">
+        <v>7.5872946013476703</v>
+      </c>
+      <c r="X7" s="5">
+        <v>1317.9022909562893</v>
+      </c>
+      <c r="Y7" s="5">
+        <v>131.73923116721156</v>
+      </c>
+      <c r="Z7" s="4">
+        <v>3004.2507321019202</v>
+      </c>
+      <c r="AA7" s="5">
+        <v>295.11424673674685</v>
+      </c>
+      <c r="AB7" s="5">
+        <v>1182.4594829924292</v>
+      </c>
+      <c r="AC7" s="5">
+        <v>19.357146226667471</v>
+      </c>
+      <c r="AD7" s="5">
+        <v>835861.90568216599</v>
+      </c>
+      <c r="AE7" s="5">
+        <v>854631.57311942684</v>
+      </c>
+      <c r="AF7" s="5">
+        <v>6996.7000245717927</v>
+      </c>
+      <c r="AG7" s="5">
+        <v>1791.5237313883033</v>
+      </c>
+      <c r="AH7" s="5">
+        <v>2643.6829523105557</v>
+      </c>
+      <c r="AI7" s="5">
+        <v>893.99144571413547</v>
+      </c>
+      <c r="AJ7" s="5">
+        <v>4052.5809998457257</v>
+      </c>
+      <c r="AK7" s="5">
+        <v>942.56403578660593</v>
+      </c>
+      <c r="AL7" s="4">
+        <v>1888.2721716865199</v>
+      </c>
+      <c r="AM7" s="4">
+        <v>96.586569116910368</v>
+      </c>
+      <c r="AN7" s="5">
+        <v>1842.1794635079682</v>
+      </c>
+      <c r="AO7" s="5">
+        <v>36.552507770680243</v>
+      </c>
+      <c r="AP7" s="5">
+        <v>79841.413565268333</v>
+      </c>
+      <c r="AQ7" s="5">
+        <v>37125.890914137119</v>
+      </c>
+      <c r="AR7" s="5">
+        <v>2280.0907047214109</v>
+      </c>
+      <c r="AS7" s="5">
+        <v>134.17500573121703</v>
+      </c>
+      <c r="AT7" s="5">
+        <v>2203.2352113342258</v>
+      </c>
+      <c r="AU7" s="5">
+        <v>53.927293179653653</v>
+      </c>
+      <c r="AV7" s="5">
+        <v>2200.0068694607671</v>
+      </c>
+      <c r="AW7" s="4">
+        <v>5.7896961919447806E-4</v>
+      </c>
+      <c r="AX7" s="5">
+        <v>2300.0070298778965</v>
+      </c>
+      <c r="AY7" s="4">
+        <v>6.7509277509934221E-4</v>
+      </c>
+      <c r="AZ7" s="5">
+        <v>2835.2361947018567</v>
+      </c>
+      <c r="BA7" s="4">
+        <v>9.4949649135044236</v>
+      </c>
+      <c r="BB7" s="5">
+        <v>3388.7108152070591</v>
+      </c>
+      <c r="BC7" s="5">
+        <v>7.5886119432393642</v>
+      </c>
+      <c r="BD7" s="4">
+        <v>2903.1410290335357</v>
+      </c>
+      <c r="BE7" s="4">
+        <v>4.3674474447989802</v>
+      </c>
+      <c r="BF7" s="4">
+        <v>4522.3415207909866</v>
+      </c>
+      <c r="BG7" s="5">
+        <v>653.03626597584696</v>
+      </c>
+      <c r="BH7" s="4">
+        <v>3437.9121909343467</v>
+      </c>
+      <c r="BI7" s="4">
+        <v>18.448554453562686</v>
+      </c>
+      <c r="BJ7" s="5">
+        <v>3234.785653591608</v>
+      </c>
+      <c r="BK7" s="4">
+        <v>22.368365960239732</v>
+      </c>
+      <c r="BL7" s="4">
+        <v>3382.156529187384</v>
+      </c>
+      <c r="BM7" s="4">
+        <v>52.750128452935591</v>
+      </c>
+      <c r="BN7" s="5">
+        <v>51505.542266634395</v>
+      </c>
+      <c r="BO7" s="5">
+        <v>20131.106921354283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:67">
+      <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="5">
@@ -994,8 +1997,8 @@
         <v>551.29800603326112</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="B9" t="s">
+    <row r="9" spans="1:67">
+      <c r="B9" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="5">
@@ -1011,11 +2014,11 @@
         <v>8.7525245576868933</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
+    <row r="10" spans="1:67">
+      <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="5">
@@ -1031,8 +2034,8 @@
         <v>604.38381426940407</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="B11" t="s">
+    <row r="11" spans="1:67">
+      <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="5">
@@ -1048,11 +2051,11 @@
         <v>1.0771803784837304</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
+    <row r="12" spans="1:67">
+      <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="5">
@@ -1068,8 +2071,8 @@
         <v>821.39183141272224</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="B13" t="s">
+    <row r="13" spans="1:67">
+      <c r="B13" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="5">
@@ -1085,11 +2088,11 @@
         <v>16.623902653343638</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
+    <row r="14" spans="1:67">
+      <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="5">
@@ -1105,8 +2108,8 @@
         <v>849.16218611826037</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="B15" t="s">
+    <row r="15" spans="1:67">
+      <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="5">
@@ -1122,11 +2125,11 @@
         <v>7.5872946013476703</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
+    <row r="16" spans="1:67">
+      <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="5">
@@ -1143,7 +2146,7 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="5">
@@ -1160,10 +2163,10 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" t="s">
+      <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="5">
@@ -1180,7 +2183,7 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C19" s="5">
@@ -1197,10 +2200,10 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" t="s">
+      <c r="A20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C20" s="4">
@@ -1217,7 +2220,7 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C21" s="4">
@@ -1234,10 +2237,10 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" t="s">
+      <c r="A22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="4">
@@ -1254,7 +2257,7 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C23" s="4">
@@ -1271,10 +2274,10 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" t="s">
+      <c r="A24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="4">
@@ -1291,7 +2294,7 @@
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="5">
@@ -1308,10 +2311,10 @@
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" t="s">
+      <c r="A26" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="5">
@@ -1328,7 +2331,7 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C27" s="5">
@@ -1345,10 +2348,10 @@
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" t="s">
+      <c r="A28" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C28" s="5">
@@ -1365,7 +2368,7 @@
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="B29" t="s">
+      <c r="B29" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C29" s="5">
@@ -1382,10 +2385,10 @@
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" t="s">
+      <c r="A30" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="5">
@@ -1402,7 +2405,7 @@
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="B31" t="s">
+      <c r="B31" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="5">
@@ -1419,10 +2422,10 @@
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" t="s">
+      <c r="A32" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="5">
@@ -1439,7 +2442,7 @@
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="B33" t="s">
+      <c r="B33" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C33" s="5">
@@ -1456,10 +2459,10 @@
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" t="s">
+      <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="5">
@@ -1476,7 +2479,7 @@
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="B35" t="s">
+      <c r="B35" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C35" s="5">
@@ -1493,10 +2496,10 @@
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" t="s">
+      <c r="A36" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C36" s="4">
@@ -1513,7 +2516,7 @@
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="B37" t="s">
+      <c r="B37" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C37" s="5">
@@ -1530,10 +2533,10 @@
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" t="s">
+      <c r="A38" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C38" s="5">
@@ -1550,7 +2553,7 @@
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="B39" t="s">
+      <c r="B39" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C39" s="5">
@@ -1567,10 +2570,10 @@
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" t="s">
+      <c r="A40" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C40" s="4">
@@ -1587,7 +2590,7 @@
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="B41" t="s">
+      <c r="B41" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C41" s="5">
@@ -1604,10 +2607,10 @@
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" t="s">
+      <c r="A42" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C42" s="5">
@@ -1624,7 +2627,7 @@
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="B43" t="s">
+      <c r="B43" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C43" s="5">
@@ -1641,10 +2644,10 @@
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" t="s">
+      <c r="A44" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C44" s="5">
@@ -1661,7 +2664,7 @@
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="B45" t="s">
+      <c r="B45" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C45" s="5">
@@ -1678,10 +2681,10 @@
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" t="s">
+      <c r="A46" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C46" s="5">
@@ -1698,7 +2701,7 @@
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="B47" t="s">
+      <c r="B47" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C47" s="5">
@@ -1715,10 +2718,10 @@
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" t="s">
+      <c r="A48" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C48" s="5">
@@ -1734,8 +2737,8 @@
         <v>2903.1410290335357</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
-      <c r="B49" t="s">
+    <row r="49" spans="1:10">
+      <c r="B49" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C49" s="5">
@@ -1751,11 +2754,11 @@
         <v>4.3674474447989802</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
-      <c r="A50" t="s">
+    <row r="50" spans="1:10">
+      <c r="A50" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C50" s="5">
@@ -1771,8 +2774,8 @@
         <v>4522.3415207909866</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
-      <c r="B51" t="s">
+    <row r="51" spans="1:10">
+      <c r="B51" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C51" s="4">
@@ -1787,12 +2790,15 @@
       <c r="F51" s="5">
         <v>653.03626597584696</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" t="s">
+      <c r="J51" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C52" s="5">
@@ -1807,9 +2813,12 @@
       <c r="F52" s="4">
         <v>3437.9121909343467</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="B53" t="s">
+      <c r="J52" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="B53" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C53" s="5">
@@ -1824,12 +2833,15 @@
       <c r="F53" s="4">
         <v>18.448554453562686</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" t="s">
+      <c r="J53" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C54" s="4">
@@ -1844,9 +2856,12 @@
       <c r="F54" s="5">
         <v>3234.785653591608</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="B55" t="s">
+      <c r="J54" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="B55" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C55" s="5">
@@ -1862,11 +2877,11 @@
         <v>22.368365960239732</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
-      <c r="A56" t="s">
+    <row r="56" spans="1:10">
+      <c r="A56" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C56" s="5">
@@ -1882,8 +2897,8 @@
         <v>3382.156529187384</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
-      <c r="B57" t="s">
+    <row r="57" spans="1:10">
+      <c r="B57" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C57" s="5">
@@ -1899,11 +2914,11 @@
         <v>52.750128452935591</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
-      <c r="A58" t="s">
+    <row r="58" spans="1:10">
+      <c r="A58" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C58" s="5">
@@ -1919,8 +2934,8 @@
         <v>51505.542266634395</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
-      <c r="B59" t="s">
+    <row r="59" spans="1:10">
+      <c r="B59" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C59" s="5">
@@ -1936,11 +2951,11 @@
         <v>20131.106921354283</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
-      <c r="A60" t="s">
+    <row r="60" spans="1:10">
+      <c r="A60" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D60" s="3" t="s">
@@ -1953,11 +2968,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
-      <c r="A61" t="s">
+    <row r="61" spans="1:10">
+      <c r="A61" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D61" s="3" t="s">
@@ -1972,6 +2987,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16770,13 +17786,15 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5703125" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="2.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="5" width="2.140625" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
@@ -17482,7 +18500,7 @@
       <c r="A32" t="s">
         <v>97</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>98</v>
       </c>
       <c r="C32" t="s">

</xml_diff>